<commit_message>
Fixed the CDN Invoice feature also fixed the order path to the invoice in teh CDN
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/OrderInvoiceTemplate.xlsx
+++ b/src/main/resources/templates/OrderInvoiceTemplate.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28318"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1A6F3CAC-21EE-4D37-921A-224343457F25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F12093BE-3E30-4A20-BE86-AD0D8C0F815A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Name of the product</t>
   </si>
@@ -42,10 +42,16 @@
     <t>Discount in %</t>
   </si>
   <si>
+    <t>Price Discount</t>
+  </si>
+  <si>
     <t>VAT</t>
   </si>
   <si>
     <t>Price with VAT</t>
+  </si>
+  <si>
+    <t>Home Elevator</t>
   </si>
 </sst>
 </file>
@@ -417,20 +423,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18.5703125" customWidth="1"/>
     <col min="3" max="3" width="13.85546875" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
+    <col min="6" max="6" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -445,6 +453,29 @@
       </c>
       <c r="E1" t="s">
         <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2">
+        <v>23440</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>20</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>